<commit_message>
adjust some cmd timeout setting
adjust some cmd timeout setting
</commit_message>
<xml_diff>
--- a/SmartTap2.1_TW/KB test case/1_Test case.xlsx
+++ b/SmartTap2.1_TW/KB test case/1_Test case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vivotech\regress\regression\regress_test\test_tree\SmartTap2.1_TW\KB test case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9E3E43-1B1C-417E-9E37-4A5A85861B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2636F8-7D9A-4261-AAD4-24CB848AF5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="90" windowWidth="15945" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="795" windowWidth="18810" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1834,7 +1834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>